<commit_message>
register competition create excel done
</commit_message>
<xml_diff>
--- a/server/רישום ספורטאים לתחרות.xlsx
+++ b/server/רישום ספורטאים לתחרות.xlsx
@@ -5,13 +5,13 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="רישום ספורטאים לתחרות" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>ת.ז ספורטאי</t>
   </si>
@@ -119,13 +119,67 @@
   </si>
   <si>
     <t>קריליוק</t>
+  </si>
+  <si>
+    <t>זכר דואן בנים 7-7 (קוד: 16)</t>
+  </si>
+  <si>
+    <t>זכר נשק קצר חלקי 8-9 (קוד: 11)</t>
+  </si>
+  <si>
+    <t>זכר צאן סואן בנים 9-12 (קוד: 15)</t>
+  </si>
+  <si>
+    <t>זכר צאן חלקי בנים 9-11 (קוד: 1)</t>
+  </si>
+  <si>
+    <t>זכר נשק ארוך בנים 10-12 (קוד: 3)</t>
+  </si>
+  <si>
+    <t>זכר נשק קצר בנים 11-11 (קוד: 8)</t>
+  </si>
+  <si>
+    <t>זכר נשק ארוך בנים 14-14 (קוד: 5)</t>
+  </si>
+  <si>
+    <t>זכר צאן חלקי בנים 14-14 (קוד: 2)</t>
+  </si>
+  <si>
+    <t>מעורב נשק ארוך 14-14 (קוד: 6)</t>
+  </si>
+  <si>
+    <t>נקבה דואילין בנות  (קוד: 18)</t>
+  </si>
+  <si>
+    <t>נקבה דואן בנות 7-7 (קוד: 17)</t>
+  </si>
+  <si>
+    <t>נקבה בלי נשק בנות 9-12 (קוד: 12)</t>
+  </si>
+  <si>
+    <t>נקבה נשק קצר בנות 9-11 (קוד: 9)</t>
+  </si>
+  <si>
+    <t>נקבה נשק ארוך בנות 10-10 (קוד: 4)</t>
+  </si>
+  <si>
+    <t>נקבה נשק ארוך חלקי 11-11 (קוד: 7)</t>
+  </si>
+  <si>
+    <t>נקבה נשק קצר בנות 14-14 (קוד: 10)</t>
+  </si>
+  <si>
+    <t>נקבה צאן סואן בנות 14-14 (קוד: 14)</t>
+  </si>
+  <si>
+    <t>נקבה בלי נשק בוגרות 18+ (קוד: 13)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -142,6 +196,12 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="1"/>
     </font>
@@ -163,17 +223,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf applyFont="1" fontId="0"/>
     <xf applyFont="1" fontId="1"/>
     <xf applyFont="1" fontId="2"/>
+    <xf applyFont="1" fontId="3" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="true" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomRight" state="frozen"/>
@@ -186,7 +249,7 @@
     <col min="8" max="8" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:26">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -211,8 +274,11 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="Z1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" s="1" t="n">
         <v>341090389</v>
       </c>
@@ -228,8 +294,11 @@
       <c r="E2" s="1" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="Z2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" s="1" t="n">
         <v>217481712</v>
       </c>
@@ -245,8 +314,11 @@
       <c r="E3" s="1" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="Z3" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" s="1" t="n">
         <v>331962472</v>
       </c>
@@ -262,8 +334,11 @@
       <c r="E4" s="1" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="Z4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" s="1" t="n">
         <v>216011056</v>
       </c>
@@ -279,8 +354,11 @@
       <c r="E5" s="1" t="n">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="Z5" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6" s="1" t="n">
         <v>215241241</v>
       </c>
@@ -296,8 +374,11 @@
       <c r="E6" s="1" t="n">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="Z6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7" s="1" t="n">
         <v>331763706</v>
       </c>
@@ -313,8 +394,11 @@
       <c r="E7" s="1" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="Z7" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
       <c r="A8" s="1" t="n">
         <v>217032051</v>
       </c>
@@ -330,8 +414,11 @@
       <c r="E8" s="1" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="Z8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9" s="1" t="n">
         <v>213186281</v>
       </c>
@@ -347,8 +434,11 @@
       <c r="E9" s="1" t="n">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="Z9" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10" s="1" t="n">
         <v>218532406</v>
       </c>
@@ -364,8 +454,11 @@
       <c r="E10" s="1" t="n">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="Z10" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
       <c r="A11" s="1" t="n">
         <v>218532407</v>
       </c>
@@ -381,8 +474,11 @@
       <c r="E11" s="1" t="n">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="Z11" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
       <c r="A12" s="1" t="n">
         <v>318896149</v>
       </c>
@@ -398,8 +494,11 @@
       <c r="E12" s="1" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="Z12" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13" s="1" t="n">
         <v>209186584</v>
       </c>
@@ -415,8 +514,11 @@
       <c r="E13" s="1" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="Z13" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
       <c r="A14" s="1" t="n">
         <v>321772782</v>
       </c>
@@ -432,17 +534,40 @@
       <c r="E14" s="1" t="n">
         <v>24</v>
       </c>
+      <c r="Z14" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="26:26">
+      <c r="Z15" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="26:26">
+      <c r="Z16" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="26:26">
+      <c r="Z17" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="26:26">
+      <c r="Z18" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid choice was chosen" prompt="בחר קטגוריה" sqref="F2:F14">
-      <formula1>",נקבה בלי נשק בוגרות 18+,נקבה בלי נשק בנות 9-12,נקבה דואילין בנות ,זכר דואילין בנים ,נקבה דואן בנות 7-7,זכר דואן בנים 7-7,מעורב נשק ארוך 14-14,נקבה נשק ארוך בנות 10-10,זכר נשק ארוך בנים 14-14,זכר נשק ארוך בנים 10-12,נקבה נשק ארוך חלקי 11-11,נקבה נשק קצר בנות 9-11,נקבה נשק קצר בנות 14-14,זכר נשק קצר בנים 11-11,זכר נשק קצר חלקי 8-9,זכר צאן חלקי בנים 9-11,זכר צאן חלקי בנים 14-14,נקבה צאן סואן בנות 14-14,זכר צאן סואן בנים 9-12"</formula1>
+    <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" error="Invalid choice was chosen" prompt="בחר קטגוריה" sqref="F2:F14">
+      <formula1>=sheet1!$Z$1:$Z$100</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid choice was chosen" prompt="בחר קטגוריה" sqref="G2:G14">
-      <formula1>",נקבה בלי נשק בוגרות 18+,נקבה בלי נשק בנות 9-12,נקבה דואילין בנות ,זכר דואילין בנים ,נקבה דואן בנות 7-7,זכר דואן בנים 7-7,מעורב נשק ארוך 14-14,נקבה נשק ארוך בנות 10-10,זכר נשק ארוך בנים 14-14,זכר נשק ארוך בנים 10-12,נקבה נשק ארוך חלקי 11-11,נקבה נשק קצר בנות 9-11,נקבה נשק קצר בנות 14-14,זכר נשק קצר בנים 11-11,זכר נשק קצר חלקי 8-9,זכר צאן חלקי בנים 9-11,זכר צאן חלקי בנים 14-14,נקבה צאן סואן בנות 14-14,זכר צאן סואן בנים 9-12"</formula1>
+    <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" error="Invalid choice was chosen" prompt="בחר קטגוריה" sqref="G2:G14">
+      <formula1>=sheet1!$Z$1:$Z$100</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid choice was chosen" prompt="בחר קטגוריה" sqref="H2:H14">
-      <formula1>""</formula1>
+    <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" error="Invalid choice was chosen" prompt="בחר קטגוריה" sqref="H2:H14">
+      <formula1>=sheet1!$Z$1:$Z$100</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>